<commit_message>
Updated data cleaning to rename Health Science to Health Sciences
</commit_message>
<xml_diff>
--- a/data/students-clean.xlsx
+++ b/data/students-clean.xlsx
@@ -3784,576 +3784,579 @@
     <t>Social Science and Humanities</t>
   </si>
   <si>
+    <t>Health Sciences</t>
+  </si>
+  <si>
+    <t>Biological Science</t>
+  </si>
+  <si>
+    <t>Life Sciences</t>
+  </si>
+  <si>
+    <t>Forensic Science</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Life Science</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>biological science</t>
+  </si>
+  <si>
+    <t>Nuclear Engineering</t>
+  </si>
+  <si>
+    <t>nuclear engineering</t>
+  </si>
+  <si>
+    <t>Radiation Science and Health Physics</t>
+  </si>
+  <si>
+    <t>medical physics and radiation science</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>Nuclear engineering</t>
+  </si>
+  <si>
+    <t>Nuclear Eng.</t>
+  </si>
+  <si>
+    <t>NuclearScience</t>
+  </si>
+  <si>
+    <t>Bachelor of Engineering</t>
+  </si>
+  <si>
+    <t>Nuclear Engineer</t>
+  </si>
+  <si>
+    <t>Health Physics and Radiation Science</t>
+  </si>
+  <si>
+    <t>Health Physics and Radiation Sciences</t>
+  </si>
+  <si>
+    <t>health physics and radiation science</t>
+  </si>
+  <si>
+    <t>BCom HR and OB</t>
+  </si>
+  <si>
+    <t>Game Development &amp; Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Commerce</t>
+  </si>
+  <si>
+    <t>entreprenureship</t>
+  </si>
+  <si>
+    <t>IT Security and Networking</t>
+  </si>
+  <si>
+    <t>Game Development</t>
+  </si>
+  <si>
+    <t>Networking and IT security</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce (Hons), Org. Behaviour &amp; Human Resources Mgmt</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce (Hons)</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Human Reslurces</t>
+  </si>
+  <si>
+    <t>game develompent</t>
+  </si>
+  <si>
+    <t>entrepreneurship</t>
+  </si>
+  <si>
+    <t>Legal Studies (Bridge) with Honors</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce, Marketing</t>
+  </si>
+  <si>
+    <t>INFORMATION TECHNOLOGY - NETWORKING AND INFORMATION TECHNOLOGY SECURITY</t>
+  </si>
+  <si>
+    <t>Networking &amp; IT Security</t>
+  </si>
+  <si>
+    <t>Commerce (Hons)</t>
+  </si>
+  <si>
+    <t>Organizational Behaviour and Human Resouce Management</t>
+  </si>
+  <si>
+    <t>BComm</t>
+  </si>
+  <si>
+    <t>Network and Information Technology Security</t>
+  </si>
+  <si>
+    <t>Information technology and network security</t>
+  </si>
+  <si>
+    <t>Bachelor of Information Technology (Hons), Networking &amp; IT Security</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce</t>
+  </si>
+  <si>
+    <t>Game Development and Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Commerce (Accounting)</t>
+  </si>
+  <si>
+    <t>Information technology and networking security</t>
+  </si>
+  <si>
+    <t>Business administration- finance</t>
+  </si>
+  <si>
+    <t>commerce</t>
+  </si>
+  <si>
+    <t>Bachelor of commerce</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce (Hons), Accounting</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Game design</t>
+  </si>
+  <si>
+    <t>Networking and IT Security</t>
+  </si>
+  <si>
+    <t>Game development and entrepreneurship</t>
+  </si>
+  <si>
+    <t>Networking and Security</t>
+  </si>
+  <si>
+    <t>Commerce - Finance</t>
+  </si>
+  <si>
+    <t>Information Technology Security and Networking</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Networking And Information Technology Security</t>
+  </si>
+  <si>
+    <t>Game Dev</t>
+  </si>
+  <si>
+    <t>Game  Development</t>
+  </si>
+  <si>
+    <t>Information Technology &amp; Networking</t>
+  </si>
+  <si>
+    <t>Bachelor of Commerce (Accounting)</t>
+  </si>
+  <si>
+    <t>Game Development and Entrepeneurship</t>
+  </si>
+  <si>
+    <t>Game development and Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Networking &amp; IT secruity</t>
+  </si>
+  <si>
+    <t>Networking &amp; I.T. Security</t>
+  </si>
+  <si>
+    <t>Bcomm Finance</t>
+  </si>
+  <si>
+    <t>Bcomm finance</t>
+  </si>
+  <si>
+    <t>IT and networking security</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Computer Networking and I.T. security</t>
+  </si>
+  <si>
+    <t>Game Developement</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>bachelor of commerce/accouonting</t>
+  </si>
+  <si>
+    <t>Game Dev &amp; Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Networking and information technology security</t>
+  </si>
+  <si>
+    <t>Accounting - Commerce</t>
+  </si>
+  <si>
+    <t>NETWORKING AND INFORMATION TECHNOLOGY SECURITY</t>
+  </si>
+  <si>
+    <t>Bachelor of I.T. - Networking &amp; I.T. Security</t>
+  </si>
+  <si>
+    <t>game development and entrepreneurship</t>
+  </si>
+  <si>
+    <t>BComm - Accounting</t>
+  </si>
+  <si>
+    <t>game development and entreperneuship</t>
+  </si>
+  <si>
+    <t>Game Development and Entreprenuership</t>
+  </si>
+  <si>
+    <t>Networking and I.T. Security</t>
+  </si>
+  <si>
+    <t>Game Development and entrepreneurship</t>
+  </si>
+  <si>
+    <t>IT and Network Security</t>
+  </si>
+  <si>
+    <t>game development and entreprenuership</t>
+  </si>
+  <si>
+    <t>It. Security</t>
+  </si>
+  <si>
+    <t>Business Commerce</t>
+  </si>
+  <si>
+    <t>networking and information technology security</t>
+  </si>
+  <si>
+    <t>Networking and IT secruity</t>
+  </si>
+  <si>
+    <t>Networking and Information Technology Security</t>
+  </si>
+  <si>
+    <t>IT and Networking Securities</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Mechatronics</t>
+  </si>
+  <si>
+    <t>mechatronic engineering</t>
+  </si>
+  <si>
+    <t>Automotive engineering</t>
+  </si>
+  <si>
+    <t>Software engineering</t>
+  </si>
+  <si>
+    <t>Electrical Engineering</t>
+  </si>
+  <si>
+    <t>Mechanical engineerimg</t>
+  </si>
+  <si>
+    <t>M.EngM</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineering</t>
+  </si>
+  <si>
+    <t>Engineering management</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Mechatronics Engineering</t>
+  </si>
+  <si>
+    <t>software engineering</t>
+  </si>
+  <si>
+    <t>MASTERS IN MECHANICAL ENGINEERING</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering - Comprehensive</t>
+  </si>
+  <si>
+    <t>Master of engineering Management</t>
+  </si>
+  <si>
+    <t>MEngg in Electrical and Computer engineering</t>
+  </si>
+  <si>
+    <t>Energy Engineering</t>
+  </si>
+  <si>
+    <t>Electrical engineering</t>
+  </si>
+  <si>
+    <t>automotive engineering</t>
+  </si>
+  <si>
+    <t>Mechatronics engineering</t>
+  </si>
+  <si>
+    <t>Mechatronics Engineering Management</t>
+  </si>
+  <si>
+    <t>M.Eng in Engineering Management</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>mechatronics engineering</t>
+  </si>
+  <si>
+    <t>Mechanical engineering</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Automotive Engineering</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Electrical Engineer</t>
+  </si>
+  <si>
+    <t>electrical Engineering</t>
+  </si>
+  <si>
+    <t>mechatronics</t>
+  </si>
+  <si>
+    <t>Mechanical Engeeniring</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>electrical engineering</t>
+  </si>
+  <si>
+    <t>mechanical engineering</t>
+  </si>
+  <si>
+    <t>Master's Enginering Management</t>
+  </si>
+  <si>
+    <t>MECHATRONICS</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Automobile Engineering</t>
+  </si>
+  <si>
+    <t>Bachelor of Mechatronics Engineering (Hons.)</t>
+  </si>
+  <si>
+    <t>Mechatronica</t>
+  </si>
+  <si>
+    <t>Software Enginerering</t>
+  </si>
+  <si>
+    <t>Mechanical Eng</t>
+  </si>
+  <si>
+    <t>electrical enginnering</t>
+  </si>
+  <si>
+    <t>Mechanical engineering.</t>
+  </si>
+  <si>
+    <t>Forensic Psychology</t>
+  </si>
+  <si>
+    <t>forensic psychology</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Criminology and Justice</t>
+  </si>
+  <si>
+    <t>Political Science</t>
+  </si>
+  <si>
+    <t>Criminology</t>
+  </si>
+  <si>
+    <t>legal studies</t>
+  </si>
+  <si>
+    <t>Forensic Psychology Bach. of Arts (Hons)</t>
+  </si>
+  <si>
+    <t>Criminology and justice</t>
+  </si>
+  <si>
+    <t>Legal studies</t>
+  </si>
+  <si>
+    <t>Forensic psychology</t>
+  </si>
+  <si>
+    <t>Forensic Psychology Bridge Program</t>
+  </si>
+  <si>
+    <t>criminology and justice</t>
+  </si>
+  <si>
+    <t>Legal Studies</t>
+  </si>
+  <si>
+    <t>Criminology and Justice program</t>
+  </si>
+  <si>
+    <t>Political science bridge</t>
+  </si>
+  <si>
+    <t>Communications and different media</t>
+  </si>
+  <si>
+    <t>COMMUNICATION AND DIGITAL MEDIA STUDIES</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Communications and Digital Media Studies</t>
+  </si>
+  <si>
+    <t>Communications and Digital Media - Bridge</t>
+  </si>
+  <si>
+    <t>Bachelor of Arts (Hons), Communication &amp; Digital Media Studies</t>
+  </si>
+  <si>
+    <t>Communications and Digital Media</t>
+  </si>
+  <si>
+    <t>Political Science Bridging Program</t>
+  </si>
+  <si>
+    <t>Criminal and Justice</t>
+  </si>
+  <si>
+    <t>Digital Media and Communications</t>
+  </si>
+  <si>
+    <t>Communications and Digital Media studies</t>
+  </si>
+  <si>
+    <t>criminology</t>
+  </si>
+  <si>
+    <t>Digital Media studies</t>
+  </si>
+  <si>
+    <t>Communication &amp; Digital Media Studies</t>
+  </si>
+  <si>
+    <t>RPN - BScN Bridge</t>
+  </si>
+  <si>
+    <t>Nursing</t>
+  </si>
+  <si>
+    <t>Medical Laboratory Science</t>
+  </si>
+  <si>
+    <t>Public Health</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Nursing RPN Bridge</t>
+  </si>
+  <si>
+    <t>bridging to registered Nurse</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Nursing</t>
+  </si>
+  <si>
+    <t>Nursing BScN</t>
+  </si>
+  <si>
+    <t>Nursing- Collaborative bscn</t>
+  </si>
+  <si>
+    <t>Kinesiology</t>
+  </si>
+  <si>
+    <t>Collaborative Nursing</t>
+  </si>
+  <si>
+    <t>Bachelor of Health Science (Honours)</t>
+  </si>
+  <si>
+    <t>Biological Science- Life Science</t>
+  </si>
+  <si>
+    <t>Heath sciences</t>
+  </si>
+  <si>
     <t>Health Science</t>
   </si>
   <si>
-    <t>Biological Science</t>
-  </si>
-  <si>
-    <t>Life Sciences</t>
-  </si>
-  <si>
-    <t>Forensic Science</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
-    <t>Life Science</t>
-  </si>
-  <si>
-    <t>Physics</t>
-  </si>
-  <si>
-    <t>biological science</t>
-  </si>
-  <si>
-    <t>Nuclear Engineering</t>
-  </si>
-  <si>
-    <t>nuclear engineering</t>
-  </si>
-  <si>
-    <t>Radiation Science and Health Physics</t>
-  </si>
-  <si>
-    <t>medical physics and radiation science</t>
-  </si>
-  <si>
-    <t>undergraduate</t>
-  </si>
-  <si>
-    <t>Nuclear engineering</t>
-  </si>
-  <si>
-    <t>Nuclear Eng.</t>
-  </si>
-  <si>
-    <t>NuclearScience</t>
-  </si>
-  <si>
-    <t>Bachelor of Engineering</t>
-  </si>
-  <si>
-    <t>Nuclear Engineer</t>
-  </si>
-  <si>
-    <t>Health Physics and Radiation Science</t>
-  </si>
-  <si>
-    <t>Health Physics and Radiation Sciences</t>
-  </si>
-  <si>
-    <t>health physics and radiation science</t>
-  </si>
-  <si>
-    <t>BCom HR and OB</t>
-  </si>
-  <si>
-    <t>Game Development &amp; Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Commerce</t>
-  </si>
-  <si>
-    <t>entreprenureship</t>
-  </si>
-  <si>
-    <t>IT Security and Networking</t>
-  </si>
-  <si>
-    <t>Game Development</t>
-  </si>
-  <si>
-    <t>Networking and IT security</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce (Hons), Org. Behaviour &amp; Human Resources Mgmt</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce (Hons)</t>
-  </si>
-  <si>
-    <t>Network Security</t>
-  </si>
-  <si>
-    <t>Human Reslurces</t>
-  </si>
-  <si>
-    <t>game develompent</t>
-  </si>
-  <si>
-    <t>entrepreneurship</t>
-  </si>
-  <si>
-    <t>Legal Studies (Bridge) with Honors</t>
-  </si>
-  <si>
-    <t>Accounting</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce, Marketing</t>
-  </si>
-  <si>
-    <t>INFORMATION TECHNOLOGY - NETWORKING AND INFORMATION TECHNOLOGY SECURITY</t>
-  </si>
-  <si>
-    <t>Networking &amp; IT Security</t>
-  </si>
-  <si>
-    <t>Commerce (Hons)</t>
-  </si>
-  <si>
-    <t>Organizational Behaviour and Human Resouce Management</t>
-  </si>
-  <si>
-    <t>BComm</t>
-  </si>
-  <si>
-    <t>Network and Information Technology Security</t>
-  </si>
-  <si>
-    <t>Information technology and network security</t>
-  </si>
-  <si>
-    <t>Bachelor of Information Technology (Hons), Networking &amp; IT Security</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce</t>
-  </si>
-  <si>
-    <t>Game Development and Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Commerce (Accounting)</t>
-  </si>
-  <si>
-    <t>Information technology and networking security</t>
-  </si>
-  <si>
-    <t>Business administration- finance</t>
-  </si>
-  <si>
-    <t>commerce</t>
-  </si>
-  <si>
-    <t>Bachelor of commerce</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce (Hons), Accounting</t>
-  </si>
-  <si>
-    <t>Human Resources</t>
-  </si>
-  <si>
-    <t>Game design</t>
-  </si>
-  <si>
-    <t>Networking and IT Security</t>
-  </si>
-  <si>
-    <t>Game development and entrepreneurship</t>
-  </si>
-  <si>
-    <t>Networking and Security</t>
-  </si>
-  <si>
-    <t>Commerce - Finance</t>
-  </si>
-  <si>
-    <t>Information Technology Security and Networking</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Networking And Information Technology Security</t>
-  </si>
-  <si>
-    <t>Game Dev</t>
-  </si>
-  <si>
-    <t>Game  Development</t>
-  </si>
-  <si>
-    <t>Information Technology &amp; Networking</t>
-  </si>
-  <si>
-    <t>Bachelor of Commerce (Accounting)</t>
-  </si>
-  <si>
-    <t>Game Development and Entrepeneurship</t>
-  </si>
-  <si>
-    <t>Game development and Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Networking &amp; IT secruity</t>
-  </si>
-  <si>
-    <t>Networking &amp; I.T. Security</t>
-  </si>
-  <si>
-    <t>Bcomm Finance</t>
-  </si>
-  <si>
-    <t>Bcomm finance</t>
-  </si>
-  <si>
-    <t>IT and networking security</t>
-  </si>
-  <si>
-    <t>Networking</t>
-  </si>
-  <si>
-    <t>Computer Networking and I.T. security</t>
-  </si>
-  <si>
-    <t>Game Developement</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>bachelor of commerce/accouonting</t>
-  </si>
-  <si>
-    <t>Game Dev &amp; Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Networking and information technology security</t>
-  </si>
-  <si>
-    <t>Accounting - Commerce</t>
-  </si>
-  <si>
-    <t>NETWORKING AND INFORMATION TECHNOLOGY SECURITY</t>
-  </si>
-  <si>
-    <t>Bachelor of I.T. - Networking &amp; I.T. Security</t>
-  </si>
-  <si>
-    <t>game development and entrepreneurship</t>
-  </si>
-  <si>
-    <t>BComm - Accounting</t>
-  </si>
-  <si>
-    <t>game development and entreperneuship</t>
-  </si>
-  <si>
-    <t>Game Development and Entreprenuership</t>
-  </si>
-  <si>
-    <t>Networking and I.T. Security</t>
-  </si>
-  <si>
-    <t>Game Development and entrepreneurship</t>
-  </si>
-  <si>
-    <t>IT and Network Security</t>
-  </si>
-  <si>
-    <t>game development and entreprenuership</t>
-  </si>
-  <si>
-    <t>It. Security</t>
-  </si>
-  <si>
-    <t>Business Commerce</t>
-  </si>
-  <si>
-    <t>networking and information technology security</t>
-  </si>
-  <si>
-    <t>Networking and IT secruity</t>
-  </si>
-  <si>
-    <t>Networking and Information Technology Security</t>
-  </si>
-  <si>
-    <t>IT and Networking Securities</t>
-  </si>
-  <si>
-    <t>Mechanical Engineering</t>
-  </si>
-  <si>
-    <t>Mechatronics</t>
-  </si>
-  <si>
-    <t>mechatronic engineering</t>
-  </si>
-  <si>
-    <t>Automotive engineering</t>
-  </si>
-  <si>
-    <t>Software engineering</t>
-  </si>
-  <si>
-    <t>Electrical Engineering</t>
-  </si>
-  <si>
-    <t>Mechanical engineerimg</t>
-  </si>
-  <si>
-    <t>M.EngM</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>Manufacturing Engineering</t>
-  </si>
-  <si>
-    <t>Engineering management</t>
-  </si>
-  <si>
-    <t>Mechanical</t>
-  </si>
-  <si>
-    <t>Mechatronics Engineering</t>
-  </si>
-  <si>
-    <t>software engineering</t>
-  </si>
-  <si>
-    <t>MASTERS IN MECHANICAL ENGINEERING</t>
-  </si>
-  <si>
-    <t>Mechanical Engineering - Comprehensive</t>
-  </si>
-  <si>
-    <t>Master of engineering Management</t>
-  </si>
-  <si>
-    <t>MEngg in Electrical and Computer engineering</t>
-  </si>
-  <si>
-    <t>Energy Engineering</t>
-  </si>
-  <si>
-    <t>Electrical engineering</t>
-  </si>
-  <si>
-    <t>automotive engineering</t>
-  </si>
-  <si>
-    <t>Mechatronics engineering</t>
-  </si>
-  <si>
-    <t>Mechatronics Engineering Management</t>
-  </si>
-  <si>
-    <t>M.Eng in Engineering Management</t>
-  </si>
-  <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
-    <t>mechatronics engineering</t>
-  </si>
-  <si>
-    <t>Mechanical engineering</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Automotive Engineering</t>
-  </si>
-  <si>
-    <t>Electrical</t>
-  </si>
-  <si>
-    <t>Automotive</t>
-  </si>
-  <si>
-    <t>Electrical Engineer</t>
-  </si>
-  <si>
-    <t>electrical Engineering</t>
-  </si>
-  <si>
-    <t>mechatronics</t>
-  </si>
-  <si>
-    <t>Mechanical Engeeniring</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>electrical engineering</t>
-  </si>
-  <si>
-    <t>mechanical engineering</t>
-  </si>
-  <si>
-    <t>Master's Enginering Management</t>
-  </si>
-  <si>
-    <t>MECHATRONICS</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Automobile Engineering</t>
-  </si>
-  <si>
-    <t>Bachelor of Mechatronics Engineering (Hons.)</t>
-  </si>
-  <si>
-    <t>Mechatronica</t>
-  </si>
-  <si>
-    <t>Software Enginerering</t>
-  </si>
-  <si>
-    <t>Mechanical Eng</t>
-  </si>
-  <si>
-    <t>electrical enginnering</t>
-  </si>
-  <si>
-    <t>Mechanical engineering.</t>
-  </si>
-  <si>
-    <t>Forensic Psychology</t>
-  </si>
-  <si>
-    <t>forensic psychology</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Criminology and Justice</t>
-  </si>
-  <si>
-    <t>Political Science</t>
-  </si>
-  <si>
-    <t>Criminology</t>
-  </si>
-  <si>
-    <t>legal studies</t>
-  </si>
-  <si>
-    <t>Forensic Psychology Bach. of Arts (Hons)</t>
-  </si>
-  <si>
-    <t>Criminology and justice</t>
-  </si>
-  <si>
-    <t>Legal studies</t>
-  </si>
-  <si>
-    <t>Forensic psychology</t>
-  </si>
-  <si>
-    <t>Forensic Psychology Bridge Program</t>
-  </si>
-  <si>
-    <t>criminology and justice</t>
-  </si>
-  <si>
-    <t>Legal Studies</t>
-  </si>
-  <si>
-    <t>Criminology and Justice program</t>
-  </si>
-  <si>
-    <t>Political science bridge</t>
-  </si>
-  <si>
-    <t>Communications and different media</t>
-  </si>
-  <si>
-    <t>COMMUNICATION AND DIGITAL MEDIA STUDIES</t>
-  </si>
-  <si>
-    <t>Communications</t>
-  </si>
-  <si>
-    <t>Communications and Digital Media Studies</t>
-  </si>
-  <si>
-    <t>Communications and Digital Media - Bridge</t>
-  </si>
-  <si>
-    <t>Bachelor of Arts (Hons), Communication &amp; Digital Media Studies</t>
-  </si>
-  <si>
-    <t>Communications and Digital Media</t>
-  </si>
-  <si>
-    <t>Political Science Bridging Program</t>
-  </si>
-  <si>
-    <t>Criminal and Justice</t>
-  </si>
-  <si>
-    <t>Digital Media and Communications</t>
-  </si>
-  <si>
-    <t>Communications and Digital Media studies</t>
-  </si>
-  <si>
-    <t>criminology</t>
-  </si>
-  <si>
-    <t>Digital Media studies</t>
-  </si>
-  <si>
-    <t>Communication &amp; Digital Media Studies</t>
-  </si>
-  <si>
-    <t>RPN - BScN Bridge</t>
-  </si>
-  <si>
-    <t>Nursing</t>
-  </si>
-  <si>
-    <t>Medical Laboratory Science</t>
-  </si>
-  <si>
-    <t>Public Health</t>
-  </si>
-  <si>
-    <t>Bachelor of Science in Nursing RPN Bridge</t>
-  </si>
-  <si>
-    <t>bridging to registered Nurse</t>
-  </si>
-  <si>
-    <t>Bachelor of Science in Nursing</t>
-  </si>
-  <si>
-    <t>Nursing BScN</t>
-  </si>
-  <si>
-    <t>Nursing- Collaborative bscn</t>
-  </si>
-  <si>
-    <t>Kinesiology</t>
-  </si>
-  <si>
-    <t>Collaborative Nursing</t>
-  </si>
-  <si>
-    <t>Bachelor of Health Science (Honours)</t>
-  </si>
-  <si>
-    <t>Biological Science- Life Science</t>
-  </si>
-  <si>
-    <t>Heath sciences</t>
-  </si>
-  <si>
     <t>Nursing - Post RPN</t>
   </si>
   <si>
@@ -4364,9 +4367,6 @@
   </si>
   <si>
     <t>Nursing (collaberative)</t>
-  </si>
-  <si>
-    <t>Health Sciences</t>
   </si>
   <si>
     <t>Allied Health Science</t>
@@ -56272,7 +56272,7 @@
         <v>1256</v>
       </c>
       <c r="D559" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E559">
         <v>2</v>
@@ -56640,7 +56640,7 @@
         <v>1256</v>
       </c>
       <c r="D563" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E563">
         <v>2</v>
@@ -56732,7 +56732,7 @@
         <v>1256</v>
       </c>
       <c r="D564" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E564">
         <v>2</v>
@@ -56916,7 +56916,7 @@
         <v>1256</v>
       </c>
       <c r="D566" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="E566">
         <v>2</v>
@@ -57376,7 +57376,7 @@
         <v>1256</v>
       </c>
       <c r="D571" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E571">
         <v>2</v>
@@ -57468,7 +57468,7 @@
         <v>1256</v>
       </c>
       <c r="D572" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E572">
         <v>2</v>
@@ -58020,7 +58020,7 @@
         <v>1256</v>
       </c>
       <c r="D578" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="E578">
         <v>2</v>
@@ -58296,7 +58296,7 @@
         <v>1256</v>
       </c>
       <c r="D581" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E581">
         <v>2</v>
@@ -58388,7 +58388,7 @@
         <v>1256</v>
       </c>
       <c r="D582" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E582">
         <v>2</v>
@@ -58572,7 +58572,7 @@
         <v>1256</v>
       </c>
       <c r="D584" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E584">
         <v>2</v>
@@ -59400,7 +59400,7 @@
         <v>1256</v>
       </c>
       <c r="D593" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E593">
         <v>2</v>
@@ -60228,7 +60228,7 @@
         <v>1256</v>
       </c>
       <c r="D602" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E602">
         <v>2</v>
@@ -61332,7 +61332,7 @@
         <v>1256</v>
       </c>
       <c r="D614" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E614">
         <v>2</v>
@@ -61884,7 +61884,7 @@
         <v>1256</v>
       </c>
       <c r="D620" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E620">
         <v>2</v>
@@ -62344,7 +62344,7 @@
         <v>1256</v>
       </c>
       <c r="D625" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E625">
         <v>2</v>
@@ -62896,7 +62896,7 @@
         <v>1256</v>
       </c>
       <c r="D631" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E631">
         <v>2</v>
@@ -63724,7 +63724,7 @@
         <v>1256</v>
       </c>
       <c r="D640" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E640">
         <v>2</v>
@@ -64184,7 +64184,7 @@
         <v>1256</v>
       </c>
       <c r="D645" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E645">
         <v>2</v>
@@ -64736,7 +64736,7 @@
         <v>1256</v>
       </c>
       <c r="D651" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E651">
         <v>2</v>
@@ -64920,7 +64920,7 @@
         <v>1256</v>
       </c>
       <c r="D653" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E653">
         <v>1</v>
@@ -65748,7 +65748,7 @@
         <v>1256</v>
       </c>
       <c r="D662" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E662">
         <v>2</v>
@@ -65932,7 +65932,7 @@
         <v>1256</v>
       </c>
       <c r="D664" t="s">
-        <v>1450</v>
+        <v>1256</v>
       </c>
       <c r="E664">
         <v>2</v>
@@ -66300,7 +66300,7 @@
         <v>1256</v>
       </c>
       <c r="D668" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E668">
         <v>2</v>
@@ -67036,7 +67036,7 @@
         <v>1256</v>
       </c>
       <c r="D676" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E676">
         <v>2</v>
@@ -70164,7 +70164,7 @@
         <v>1256</v>
       </c>
       <c r="D710" t="s">
-        <v>1256</v>
+        <v>1446</v>
       </c>
       <c r="E710">
         <v>2</v>

</xml_diff>